<commit_message>
improve form control alternatives example
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/ui-controls.xlsx
+++ b/src/main/webapp/WEB-INF/books/ui-controls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F33937-EC63-B84C-85EA-A25476AB3BEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBC6E28-1F8F-FC4C-8CE0-D3CBFEBCD7CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{06F9297C-FEF9-C940-8E3C-658877237F8C}"/>
+    <workbookView xWindow="37660" yWindow="1420" windowWidth="27640" windowHeight="16940" xr2:uid="{06F9297C-FEF9-C940-8E3C-658877237F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>✔ OK</t>
   </si>
@@ -54,22 +54,16 @@
     <t>Radio Button</t>
   </si>
   <si>
-    <t>◎</t>
-  </si>
-  <si>
     <t>◉</t>
   </si>
   <si>
-    <t>🔘</t>
-  </si>
-  <si>
-    <t>⊙</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
     <t>Checkmark</t>
+  </si>
+  <si>
+    <t>○</t>
   </si>
 </sst>
 </file>
@@ -109,18 +103,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
@@ -131,6 +113,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -288,22 +284,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +617,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -632,7 +628,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" customHeight="1" thickBot="1">
@@ -669,7 +665,7 @@
     </row>
     <row r="12" spans="1:2" ht="18" thickTop="1" thickBot="1"/>
     <row r="13" spans="1:2" ht="28" thickTop="1" thickBot="1">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -678,16 +674,16 @@
     </row>
     <row r="15" spans="1:2" ht="26">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="21">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="21">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -696,25 +692,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="20">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="28">
-      <c r="A20" s="9" t="s">
-        <v>10</v>
+    <row r="20" spans="1:1" ht="29">
+      <c r="A20" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="23">
-      <c r="A21" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="A21" s="9"/>
     </row>
     <row r="22" spans="1:1" ht="31">
-      <c r="A22" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>